<commit_message>
Updates to visualization functions
</commit_message>
<xml_diff>
--- a/Metrics_SL/FeatureList.xlsx
+++ b/Metrics_SL/FeatureList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stlue\OneDrive\PostDoc UCLA\1 Post Doc UCLA\Matlab analysis\MACKtrack_SL\Metrics_SL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74767E10-652E-43A0-BBF6-21E39FD7BFE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304989F3-9382-4FD9-9E44-826425B3CA86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5F929B23-F458-4D8B-B78C-429BE10A0AF8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5F929B23-F458-4D8B-B78C-429BE10A0AF8}"/>
   </bookViews>
   <sheets>
     <sheet name="FeatureList" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="167">
   <si>
     <t>Feature Name</t>
   </si>
@@ -533,6 +533,12 @@
   </si>
   <si>
     <t>max_pos_integral_ktr</t>
+  </si>
+  <si>
+    <t>duration_ktr(:,3)</t>
+  </si>
+  <si>
+    <t>duration_nfkb(:,3)</t>
   </si>
 </sst>
 </file>
@@ -3203,10 +3209,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89338D9F-55EC-4FE0-B42E-A298036D8B23}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3266,6 +3272,11 @@
         <v>32</v>
       </c>
     </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>165</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3273,10 +3284,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16A5200F-9521-4BFF-99DB-5E18BED43D86}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A1:A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3334,6 +3345,11 @@
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>